<commit_message>
submit change member contact
</commit_message>
<xml_diff>
--- a/member/memberContact.xlsx
+++ b/member/memberContact.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -87,20 +88,20 @@
     <t>Member</t>
   </si>
   <si>
-    <t>minhquyse1995@gmail.com</t>
-  </si>
-  <si>
     <t>PusHGoD</t>
   </si>
   <si>
-    <t xml:space="preserve">truonghuuthanh95@gmail.com </t>
+    <t>truonghuuthanh95</t>
+  </si>
+  <si>
+    <t>quymm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +133,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,8 +179,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
@@ -463,7 +470,7 @@
   <dimension ref="A3:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,25 +481,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="C4" t="s">
@@ -506,7 +513,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
       <c r="B5" t="s">
@@ -518,15 +525,15 @@
       <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>22</v>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
       <c r="B6" t="s">
@@ -538,15 +545,15 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="F6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -559,14 +566,14 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
       <c r="B8" t="s">
@@ -584,9 +591,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1"/>
-    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId1" display="minhquyse1995@gmail.com"/>
+    <hyperlink ref="E6" r:id="rId2" display="truonghuuthanh95@gmail.com "/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>